<commit_message>
Add metadata mapping for samples
</commit_message>
<xml_diff>
--- a/digitaltwins/resources/version_2_0_0/element_mapping.xlsx
+++ b/digitaltwins/resources/version_2_0_0/element_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clin864\ctt_group\digital-twin-platform\dtp\gen3\resources\version_2_0_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clin864\ctt_group\digitaltwins-api\digitaltwins\resources\version_2_0_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99776320-9440-44C0-8C05-60CAF715CDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BEE6D1-1AE2-4CB0-AB35-02E74915E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3204" yWindow="17064" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3204" yWindow="17172" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_description" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="172">
   <si>
     <t>subject_id</t>
   </si>
@@ -49,27 +49,12 @@
     <t>Example</t>
   </si>
   <si>
-    <t>pool-1</t>
-  </si>
-  <si>
-    <t>4 weeks</t>
-  </si>
-  <si>
     <t>strain</t>
   </si>
   <si>
-    <t>sub-1</t>
-  </si>
-  <si>
     <t>pool_id</t>
   </si>
   <si>
-    <t>experimental group</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -79,168 +64,42 @@
     <t>age</t>
   </si>
   <si>
-    <t>Age of the subject (e.g., hours, days, weeks, years old) or if unknown fill in with “unknown”</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
-    <t>Sex of the subject, or if unknown fill in with “Unknown”</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
-    <t>Subject species</t>
-  </si>
-  <si>
-    <t>Rattus norvegicus</t>
-  </si>
-  <si>
-    <t>Organism strain of the subject</t>
-  </si>
-  <si>
-    <t>Sprague-Dawley</t>
-  </si>
-  <si>
     <t>RRID for strain</t>
   </si>
   <si>
-    <t>RRID:RGD_10395233</t>
-  </si>
-  <si>
     <t>age category</t>
   </si>
   <si>
     <t>age range (min)</t>
   </si>
   <si>
-    <t>The minimal age (youngest) of the research subjects. The format for this field: numerical value + space + unit (spelled out)</t>
-  </si>
-  <si>
-    <t>prime adult stage</t>
-  </si>
-  <si>
-    <t>10 days</t>
-  </si>
-  <si>
-    <t>The maximal age (oldest) of the research subjects. The format for this field: numerical value + space + unit (spelled out)</t>
-  </si>
-  <si>
-    <t>20 days</t>
-  </si>
-  <si>
     <t>age range (max)</t>
   </si>
   <si>
     <t>handedness</t>
   </si>
   <si>
-    <t>Preference of the subject to use the right or left hand, if applicable</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
     <t>genotype</t>
   </si>
   <si>
-    <t>Ignore if RRID is filled in, Genetic makeup of genetically modified alleles in transgenic animals belonging to the same subject group</t>
-  </si>
-  <si>
-    <t>MGI:3851780</t>
-  </si>
-  <si>
     <t>reference atlas</t>
   </si>
   <si>
-    <t>The reference atlas and organ</t>
-  </si>
-  <si>
     <t>protocol title</t>
   </si>
   <si>
-    <t>Once the research protocol is uploaded to Protocols.io, the title of the protocol within Protocols.io must be noted in this field.</t>
-  </si>
-  <si>
-    <t>Spinal Cord extraction</t>
-  </si>
-  <si>
-    <t>protocol.io location</t>
-  </si>
-  <si>
-    <t>The Protocol.io URL for the protocol. Once the protocol is uploaded to Protocols.io, the protocol must be shared with the SPARC group and the Protocol.io URL is noted in this field. Please share with the SPARC group.</t>
-  </si>
-  <si>
-    <t>experimental log file name</t>
-  </si>
-  <si>
-    <t>A file containing experimental records for each sample.</t>
-  </si>
-  <si>
     <t>sample_id</t>
   </si>
   <si>
     <t>wasDerivedFromSample</t>
   </si>
   <si>
-    <t>Lab-based schema for identifying each subject</t>
-  </si>
-  <si>
-    <t>Lab-based schema for identifying each sample, must be unique</t>
-  </si>
-  <si>
-    <t>sub-1_sam-2</t>
-  </si>
-  <si>
-    <t>sample_id of the sample from which the current sample was derived (e.g., slice, tissue punch, biopsy, etc.)</t>
-  </si>
-  <si>
-    <t>sub-1_sam-1</t>
-  </si>
-  <si>
-    <t>If data is collected on multiple samples at the same time include the identifier of the pool where the data file will be found.</t>
-  </si>
-  <si>
-    <t>Experimental group subject is assigned to in research project. If you have experimental groups for samples please add another column.</t>
-  </si>
-  <si>
-    <t>specimen type</t>
-  </si>
-  <si>
-    <t>specimen anatomica location</t>
-  </si>
-  <si>
-    <t>Physical type of the specimen from which the data were extracted</t>
-  </si>
-  <si>
-    <t>tissue</t>
-  </si>
-  <si>
-    <t>The organ, or subregion of organ from which the data were extracted</t>
-  </si>
-  <si>
-    <t>dentate gyrus</t>
-  </si>
-  <si>
-    <t>Additional Fields (e.g. MINDS)</t>
-  </si>
-  <si>
-    <t>Qualitative description of age category derived from UBERON life cycle stage</t>
-  </si>
-  <si>
-    <t>RRID for the strain For this field</t>
-  </si>
-  <si>
-    <t>Paxinos Rat V3</t>
-  </si>
-  <si>
-    <t>https://www.protocols.io/view/corcheapaper-based-microfluidic-device-vtwe6pe</t>
-  </si>
-  <si>
     <t>SPARC Award number</t>
   </si>
   <si>
@@ -265,12 +124,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -700,6 +553,54 @@
   </si>
   <si>
     <t>Number of samples</t>
+  </si>
+  <si>
+    <t>sample id</t>
+  </si>
+  <si>
+    <t>was derived from</t>
+  </si>
+  <si>
+    <t>sample experimental group</t>
+  </si>
+  <si>
+    <t>sample type</t>
+  </si>
+  <si>
+    <t>sample anatomical location</t>
+  </si>
+  <si>
+    <t>date of derivation</t>
+  </si>
+  <si>
+    <t>pathology</t>
+  </si>
+  <si>
+    <t>laterality</t>
+  </si>
+  <si>
+    <t>cell type</t>
+  </si>
+  <si>
+    <t>plane of section</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>cell_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_experimental_group	</t>
+  </si>
+  <si>
+    <t>date_of_derivation</t>
+  </si>
+  <si>
+    <t>plane_of_section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_anatomical_location	</t>
   </si>
 </sst>
 </file>
@@ -751,13 +652,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1041,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF15833-15E3-4C5F-A498-645F4E950DA0}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:B48"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1054,386 +954,386 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="3" customFormat="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1460,15 +1360,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1476,210 +1376,210 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1711,158 +1611,158 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1874,405 +1774,184 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94F0A20-E7B3-4D8E-AFE6-0B7E0317ACF6}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
       <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" xr:uid="{538116BF-51C0-412F-A62B-FF9678A9225E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2281,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B1071E-6A8B-4F58-AAB3-90A284CB5C0C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2296,13 +1975,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2313,44 +1992,44 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for querying samples
</commit_message>
<xml_diff>
--- a/digitaltwins/resources/version_2_0_0/element_mapping.xlsx
+++ b/digitaltwins/resources/version_2_0_0/element_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clin864\ctt_group\digitaltwins-api\digitaltwins\resources\version_2_0_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BEE6D1-1AE2-4CB0-AB35-02E74915E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348D6DF6-684C-4048-AD60-551DCAFE2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3204" yWindow="17172" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3204" yWindow="17172" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_description" sheetId="4" r:id="rId1"/>
@@ -591,16 +591,16 @@
     <t>cell_type</t>
   </si>
   <si>
-    <t xml:space="preserve">sample_experimental_group	</t>
-  </si>
-  <si>
     <t>date_of_derivation</t>
   </si>
   <si>
     <t>plane_of_section</t>
   </si>
   <si>
-    <t xml:space="preserve">sample_anatomical_location	</t>
+    <t>sample_experimental_group</t>
+  </si>
+  <si>
+    <t>sample_anatomical_location</t>
   </si>
 </sst>
 </file>
@@ -1776,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94F0A20-E7B3-4D8E-AFE6-0B7E0317ACF6}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1832,7 +1832,7 @@
         <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1880,7 +1880,7 @@
         <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1928,7 +1928,7 @@
         <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1960,7 +1960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B1071E-6A8B-4F58-AAB3-90A284CB5C0C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>

</xml_diff>